<commit_message>
Make formatting copy forever.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/test_data.xlsx
+++ b/DECS Excel Add-Ins/test files/test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9219D223-FF33-43C7-B2CE-415404809C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969D9AF-0445-400A-9D4C-18DEF686555E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t>MRN</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>REPORT DATE</t>
+  </si>
+  <si>
+    <t>Ok to update</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -131,6 +134,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,19 +588,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EEE2AD-3FF4-4EEA-86CE-ED2D8F9BD38A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,11 +610,14 @@
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1234567</v>
       </c>
@@ -620,11 +627,14 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>37250</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>23456789</v>
       </c>
@@ -634,11 +644,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>36525.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3456789</v>
       </c>
@@ -648,11 +661,14 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>41653</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>45678901</v>
       </c>
@@ -662,12 +678,12 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>39270</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
+      <c r="E5">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>